<commit_message>
Added datasheets, finalized final_BOM
</commit_message>
<xml_diff>
--- a/Documentation/aux_system/Accelerometer_BOM.xlsx
+++ b/Documentation/aux_system/Accelerometer_BOM.xlsx
@@ -12,7 +12,6 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -557,7 +556,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,11 +1212,12 @@
     <hyperlink ref="E6" r:id="rId13" display="http://www.digikey.com/product-detail/en/0022012027/WM2011-ND/171991"/>
     <hyperlink ref="G6" r:id="rId14" display="http://www.digikey.com/product-detail/en/0022012027/WM2011-ND/171991"/>
     <hyperlink ref="H6" r:id="rId15"/>
+    <hyperlink ref="H2" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId16"/>
+  <pageSetup orientation="portrait" r:id="rId17"/>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>